<commit_message>
Zadanie nr 6 jest domowe
</commit_message>
<xml_diff>
--- a/Normalizacja.xlsx
+++ b/Normalizacja.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s-121-10\Desktop\ModelowanieDanych\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4be20116ea0b14e8/Pulpit/ModelowanieDanych/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44CF3317-5BAA-4C69-A279-D4D5D7019A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="520" documentId="13_ncr:1_{44CF3317-5BAA-4C69-A279-D4D5D7019A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82CC87C4-FD3D-44A8-B24F-FFF05CB5C66D}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{657ACE6D-A815-4329-8243-94C3C670810B}"/>
+    <workbookView xWindow="11712" yWindow="0" windowWidth="11424" windowHeight="12336" activeTab="2" xr2:uid="{657ACE6D-A815-4329-8243-94C3C670810B}"/>
   </bookViews>
   <sheets>
     <sheet name="1NF" sheetId="1" r:id="rId1"/>
+    <sheet name="2NF" sheetId="2" r:id="rId2"/>
+    <sheet name="3NF" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="44">
   <si>
     <t>Miasto</t>
   </si>
@@ -78,9 +80,6 @@
     <t>economy</t>
   </si>
   <si>
-    <t>connections_count</t>
-  </si>
-  <si>
     <t>FRA</t>
   </si>
   <si>
@@ -91,6 +90,84 @@
   </si>
   <si>
     <t>datetime</t>
+  </si>
+  <si>
+    <t>AMS</t>
+  </si>
+  <si>
+    <t>JFK</t>
+  </si>
+  <si>
+    <t>JKF</t>
+  </si>
+  <si>
+    <t>DEN</t>
+  </si>
+  <si>
+    <t>connections_order</t>
+  </si>
+  <si>
+    <t>JDK</t>
+  </si>
+  <si>
+    <t>connection</t>
+  </si>
+  <si>
+    <t>Tickets</t>
+  </si>
+  <si>
+    <t>flight_id</t>
+  </si>
+  <si>
+    <t>flights</t>
+  </si>
+  <si>
+    <t>Tytuł</t>
+  </si>
+  <si>
+    <t>Reżyser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Długość </t>
+  </si>
+  <si>
+    <t>Rok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Osoba </t>
+  </si>
+  <si>
+    <t>Randy</t>
+  </si>
+  <si>
+    <t>Howard</t>
+  </si>
+  <si>
+    <t>Anthony</t>
+  </si>
+  <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t>Henry</t>
+  </si>
+  <si>
+    <t>Triple Jeopardy</t>
+  </si>
+  <si>
+    <t>Maximum Overkill</t>
+  </si>
+  <si>
+    <t>Inferno of Assassination</t>
+  </si>
+  <si>
+    <t>Jodi Tyler</t>
+  </si>
+  <si>
+    <t>Isabel Cooper</t>
+  </si>
+  <si>
+    <t>Eric Horton</t>
   </si>
 </sst>
 </file>
@@ -116,7 +193,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -135,8 +212,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -325,11 +408,56 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -364,6 +492,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -373,25 +504,55 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="22" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -412,9 +573,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office 2013–2022">
   <a:themeElements>
-    <a:clrScheme name="Pakiet Office">
+    <a:clrScheme name="Pakiet Office 2013–2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -452,7 +613,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pakiet Office">
+    <a:fontScheme name="Pakiet Office 2013–2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -558,7 +719,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pakiet Office">
+    <a:fmtScheme name="Pakiet Office 2013–2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -700,7 +861,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -708,39 +869,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77E8C2E3-1F56-480F-B33F-A17CAD7F2F14}">
-  <dimension ref="B1:L9"/>
+  <dimension ref="B1:R17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="12" t="s">
+    <row r="1" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="14"/>
-      <c r="G2" s="15" t="s">
+      <c r="C2" s="14"/>
+      <c r="D2" s="15"/>
+      <c r="F2" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-    </row>
-    <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="34"/>
+      <c r="L2" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="34"/>
+    </row>
+    <row r="3" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="11" t="s">
         <v>0</v>
       </c>
@@ -750,29 +924,44 @@
       <c r="D3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="L3" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="N3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" s="16" t="s">
+      <c r="O3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="L3" s="20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="R3" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B4" s="8" t="s">
         <v>2</v>
       </c>
@@ -782,29 +971,44 @@
       <c r="D4" s="10">
         <v>1</v>
       </c>
-      <c r="F4" s="21">
-        <v>1</v>
-      </c>
-      <c r="G4" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4" s="23" t="s">
+      <c r="F4" s="28">
+        <v>1</v>
+      </c>
+      <c r="G4" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="17" t="s">
+      <c r="I4" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="17">
-        <v>1</v>
-      </c>
-      <c r="K4" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="L4" s="22">
-        <v>45407.479166666664</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J4" s="31">
+        <v>45407.479166666664</v>
+      </c>
+      <c r="L4" s="28">
+        <v>1</v>
+      </c>
+      <c r="M4" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="N4" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="O4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="P4" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="R4" s="31">
+        <v>45407.479166666664</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
@@ -814,133 +1018,1051 @@
       <c r="D5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="21">
-        <v>2</v>
-      </c>
-      <c r="G5" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="H5" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="I5" s="17" t="s">
+      <c r="F5" s="22">
+        <v>2</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="23">
+        <v>45407.590277777781</v>
+      </c>
+      <c r="L5" s="22">
+        <v>2</v>
+      </c>
+      <c r="M5" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="N5" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="P5" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="R5" s="23">
+        <v>45407.590277777781</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B6" s="3"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="4"/>
+      <c r="F6" s="22">
+        <v>2</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="23">
+        <v>45407.479166666664</v>
+      </c>
+      <c r="L6" s="22">
+        <v>2</v>
+      </c>
+      <c r="M6" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="N6" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="P6" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="R6" s="23">
+        <v>45407.479166666664</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B7" s="3"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="4"/>
+      <c r="F7" s="22">
+        <v>2</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="23">
+        <v>45407.479166666664</v>
+      </c>
+      <c r="L7" s="22">
+        <v>2</v>
+      </c>
+      <c r="M7" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="N7" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P7" s="2">
+        <v>3</v>
+      </c>
+      <c r="Q7" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="R7" s="23">
+        <v>45407.479166666664</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B8" s="3"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="4"/>
+      <c r="F8" s="22">
+        <v>2</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="23">
+        <v>45408.479166666664</v>
+      </c>
+      <c r="L8" s="22">
+        <v>3</v>
+      </c>
+      <c r="M8" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="N8" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="P8" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="R8" s="23">
+        <v>45407.465277777781</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="17">
-        <v>3</v>
-      </c>
-      <c r="K5" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="L5" s="22">
+      <c r="F9" s="22">
+        <v>3</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" s="23">
         <v>45407.465277777781</v>
       </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="L9" s="22">
+        <v>3</v>
+      </c>
+      <c r="M9" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="N9" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P9" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="R9" s="23">
+        <v>45407.479166666664</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B10" s="3"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="4"/>
+      <c r="F10" s="22">
+        <v>3</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" s="23">
+        <v>45407.479166666664</v>
+      </c>
+      <c r="L10" s="22">
+        <v>3</v>
+      </c>
+      <c r="M10" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="N10" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P10" s="2">
+        <v>3</v>
+      </c>
+      <c r="Q10" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="R10" s="23">
+        <v>45407.479166666664</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B11" s="3"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="4"/>
+      <c r="F11" s="22">
+        <v>3</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="J11" s="23">
+        <v>45407.479166666664</v>
+      </c>
+      <c r="L11" s="22">
+        <v>4</v>
+      </c>
+      <c r="M11" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="N11" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P11" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="R11" s="23">
+        <v>45407.479166666664</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B12" s="3"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="4"/>
+      <c r="F12" s="22">
+        <v>3</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="I12" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="J12" s="23">
+        <v>45407.479166666664</v>
+      </c>
+      <c r="L12" s="22">
+        <v>5</v>
+      </c>
+      <c r="M12" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="N12" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="P12" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="R12" s="23">
+        <v>45407.465277777781</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="4">
+        <v>1</v>
+      </c>
+      <c r="F13" s="22">
+        <v>4</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="I13" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="J13" s="23">
+        <v>45407.479166666664</v>
+      </c>
+      <c r="L13" s="22">
+        <v>5</v>
+      </c>
+      <c r="M13" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="N13" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P13" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q13" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="R13" s="23">
+        <v>45407.479166666664</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="21">
-        <v>3</v>
-      </c>
-      <c r="G6" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="H6" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="I6" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="J6" s="17">
-        <v>3</v>
-      </c>
-      <c r="K6" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="L6" s="22">
+      <c r="F14" s="22">
+        <v>5</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="H14" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="J14" s="23">
         <v>45407.465277777781</v>
       </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="4">
-        <v>1</v>
-      </c>
-      <c r="F7" s="21">
-        <v>4</v>
-      </c>
-      <c r="G7" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="H7" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="I7" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7" s="17">
-        <v>1</v>
-      </c>
-      <c r="K7" s="19" t="s">
+      <c r="L14" s="24">
+        <v>5</v>
+      </c>
+      <c r="M14" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="N14" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="O14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="P14" s="6">
+        <v>3</v>
+      </c>
+      <c r="Q14" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="L7" s="22">
-        <v>45407.479166666664</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" s="21">
-        <v>5</v>
-      </c>
-      <c r="G8" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="H8" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="I8" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="J8" s="17">
-        <v>3</v>
-      </c>
-      <c r="K8" s="19" t="s">
+      <c r="R14" s="27">
+        <v>45407.479166666664</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="F15" s="22">
+        <v>5</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="L8" s="22">
-        <v>45407.465277777781</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F9" s="1"/>
+      <c r="J15" s="23">
+        <v>45407.479166666664</v>
+      </c>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="17"/>
+      <c r="P15" s="17"/>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="19"/>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="F16" s="22">
+        <v>5</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="I16" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="J16" s="23">
+        <v>45407.479166666664</v>
+      </c>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
+      <c r="Q16" s="18"/>
+      <c r="R16" s="19"/>
+    </row>
+    <row r="17" spans="6:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F17" s="24">
+        <v>5</v>
+      </c>
+      <c r="G17" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="I17" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="J17" s="27">
+        <v>45407.479166666664</v>
+      </c>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="18"/>
+      <c r="P17" s="18"/>
+      <c r="Q17" s="18"/>
+      <c r="R17" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B2:D2"/>
-    <mergeCell ref="G2:K2"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="L2:R2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E21AE58-9D98-4B8A-9A51-4819FB497879}">
+  <dimension ref="B2:R14"/>
+  <sheetViews>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B2" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="G2" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="K2" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="P2" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="37"/>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="K3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="N3" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="P3" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="R3" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B4" s="35">
+        <v>1</v>
+      </c>
+      <c r="C4" s="35">
+        <v>1</v>
+      </c>
+      <c r="D4" s="35">
+        <v>1</v>
+      </c>
+      <c r="E4" s="36">
+        <v>45407.479166666664</v>
+      </c>
+      <c r="G4" s="35">
+        <v>1</v>
+      </c>
+      <c r="H4" s="35">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="1"/>
+      <c r="K4" s="35">
+        <v>1</v>
+      </c>
+      <c r="L4" s="35">
+        <v>1</v>
+      </c>
+      <c r="M4" s="38">
+        <v>45407.479166666664</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P4" s="35">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="R4" s="17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B5" s="35">
+        <v>2</v>
+      </c>
+      <c r="C5" s="35">
+        <v>2</v>
+      </c>
+      <c r="D5" s="35">
+        <v>1</v>
+      </c>
+      <c r="E5" s="36">
+        <v>45407.590277777781</v>
+      </c>
+      <c r="G5" s="35">
+        <v>2</v>
+      </c>
+      <c r="H5" s="35">
+        <v>1</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="1"/>
+      <c r="K5" s="35">
+        <v>2</v>
+      </c>
+      <c r="L5" s="35">
+        <v>2</v>
+      </c>
+      <c r="M5" s="38">
+        <v>45407.590277777781</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P5" s="35">
+        <v>2</v>
+      </c>
+      <c r="Q5" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="R5" s="17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B6" s="35">
+        <v>2</v>
+      </c>
+      <c r="C6" s="35">
+        <v>2</v>
+      </c>
+      <c r="D6" s="35">
+        <v>2</v>
+      </c>
+      <c r="E6" s="36">
+        <v>45407.479166666664</v>
+      </c>
+      <c r="G6" s="35">
+        <v>2</v>
+      </c>
+      <c r="H6" s="35">
+        <v>2</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="1"/>
+      <c r="K6" s="35">
+        <v>3</v>
+      </c>
+      <c r="L6" s="35">
+        <v>2</v>
+      </c>
+      <c r="M6" s="38">
+        <v>45407.465277777781</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P6" s="17"/>
+      <c r="Q6" s="17"/>
+      <c r="R6" s="17"/>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B7" s="35">
+        <v>2</v>
+      </c>
+      <c r="C7" s="35">
+        <v>2</v>
+      </c>
+      <c r="D7" s="35">
+        <v>3</v>
+      </c>
+      <c r="E7" s="36">
+        <v>45407.479166666664</v>
+      </c>
+      <c r="G7" s="35">
+        <v>2</v>
+      </c>
+      <c r="H7" s="35">
+        <v>3</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="1"/>
+      <c r="K7" s="35">
+        <v>4</v>
+      </c>
+      <c r="L7" s="35">
+        <v>1</v>
+      </c>
+      <c r="M7" s="38">
+        <v>45407.479166666664</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="17"/>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B8" s="35">
+        <v>3</v>
+      </c>
+      <c r="C8" s="35">
+        <v>2</v>
+      </c>
+      <c r="D8" s="35">
+        <v>1</v>
+      </c>
+      <c r="E8" s="36">
+        <v>45407.465277777781</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="35">
+        <v>5</v>
+      </c>
+      <c r="L8" s="35">
+        <v>2</v>
+      </c>
+      <c r="M8" s="38">
+        <v>45407.465277777781</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B9" s="35">
+        <v>3</v>
+      </c>
+      <c r="C9" s="35">
+        <v>2</v>
+      </c>
+      <c r="D9" s="35">
+        <v>2</v>
+      </c>
+      <c r="E9" s="36">
+        <v>45407.479166666664</v>
+      </c>
+      <c r="H9" s="17"/>
+      <c r="I9" s="1"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="19"/>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B10" s="35">
+        <v>3</v>
+      </c>
+      <c r="C10" s="35">
+        <v>2</v>
+      </c>
+      <c r="D10" s="35">
+        <v>3</v>
+      </c>
+      <c r="E10" s="36">
+        <v>45407.479166666664</v>
+      </c>
+      <c r="H10" s="17"/>
+      <c r="I10" s="1"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="19"/>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B11" s="35">
+        <v>4</v>
+      </c>
+      <c r="C11" s="35">
+        <v>1</v>
+      </c>
+      <c r="D11" s="35">
+        <v>1</v>
+      </c>
+      <c r="E11" s="36">
+        <v>45407.479166666664</v>
+      </c>
+      <c r="H11" s="17"/>
+      <c r="I11" s="1"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="19"/>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B12" s="35">
+        <v>5</v>
+      </c>
+      <c r="C12" s="35">
+        <v>2</v>
+      </c>
+      <c r="D12" s="35">
+        <v>1</v>
+      </c>
+      <c r="E12" s="36">
+        <v>45407.465277777781</v>
+      </c>
+      <c r="H12" s="17"/>
+      <c r="I12" s="1"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="19"/>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B13" s="35">
+        <v>5</v>
+      </c>
+      <c r="C13" s="35">
+        <v>2</v>
+      </c>
+      <c r="D13" s="35">
+        <v>2</v>
+      </c>
+      <c r="E13" s="36">
+        <v>45407.479166666664</v>
+      </c>
+      <c r="H13" s="17"/>
+      <c r="I13" s="1"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="19"/>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B14" s="35">
+        <v>5</v>
+      </c>
+      <c r="C14" s="35">
+        <v>2</v>
+      </c>
+      <c r="D14" s="35">
+        <v>3</v>
+      </c>
+      <c r="E14" s="36">
+        <v>45407.479166666664</v>
+      </c>
+      <c r="H14" s="17"/>
+      <c r="I14" s="1"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="P2:R2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20DE2DF9-0865-452E-8572-DCEC06A0DA41}">
+  <dimension ref="B3:H8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B3" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B4" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="1">
+        <v>127</v>
+      </c>
+      <c r="H4" s="1">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B5" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="1">
+        <v>174</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1998</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B6" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="1">
+        <v>210</v>
+      </c>
+      <c r="H6" s="1">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B8" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>